<commit_message>
git usermanual,userstory file added
</commit_message>
<xml_diff>
--- a/src/test/resources/Data.xlsx
+++ b/src/test/resources/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\selenium\OfflineWebsiteJBK\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E47A6B-FE1B-4B9F-8F81-C77C39720E44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AA8C30-389C-4AF2-A625-6671A9FF3AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="9" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,8 @@
     <sheet name="courses" sheetId="20" r:id="rId13"/>
     <sheet name="moreinfo" sheetId="19" r:id="rId14"/>
     <sheet name="subcourses" sheetId="18" r:id="rId15"/>
-    <sheet name="Sheet2" sheetId="21" r:id="rId16"/>
-    <sheet name="Sheet1" sheetId="17" r:id="rId17"/>
+    <sheet name="whatsappOnly" sheetId="21" r:id="rId16"/>
+    <sheet name="downCol3" sheetId="17" r:id="rId17"/>
     <sheet name="statelist" sheetId="13" r:id="rId18"/>
     <sheet name="operatorHeader" sheetId="7" r:id="rId19"/>
     <sheet name="adduser" sheetId="2" r:id="rId20"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="111">
   <si>
     <t>Username</t>
   </si>
@@ -377,6 +377,9 @@
   </si>
   <si>
     <t>69.0</t>
+  </si>
+  <si>
+    <t>Prefer way</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1142,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1466,24 +1469,145 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F8FBEB-4BC5-4B08-A066-9D7AA524A9E5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308E443D-BF54-43E0-9FED-8FB576E381A7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="30.109375" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="35">
+        <v>1.8</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="35"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="35"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="35"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2263,7 +2387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E26E5B-9439-4EF2-AC40-70C306518C29}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -2396,7 +2520,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>